<commit_message>
Prevent augmented rhombohedral angles from being above 120 degrees. Add validation for rhombohedral reindexing
</commit_message>
<xml_diff>
--- a/data/GroupSpec_hexagonal.xlsx
+++ b/data/GroupSpec_hexagonal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DWMoreau/MLI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE150B1-9F45-9247-8D93-67C2B06B2C72}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A7719D-C3E7-0D4A-A219-89211174879A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="-18380" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{4239A55F-B6A0-B74B-A834-7472AF0EB929}"/>
+    <workbookView xWindow="2280" yWindow="1680" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{4239A55F-B6A0-B74B-A834-7472AF0EB929}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -1324,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B2593AE-0613-FF49-AEF2-84AD3D0B1DD3}">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54:C60"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Initial commit for the big refactoring.  - Improved dataset generation  - Random unit cell generator  - Changes to Indexing.py to support indexing by Bravais Lattice
</commit_message>
<xml_diff>
--- a/data/GroupSpec_hexagonal.xlsx
+++ b/data/GroupSpec_hexagonal.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DWMoreau/MLI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A7719D-C3E7-0D4A-A219-89211174879A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628C3B28-0E76-1C41-B258-74FF8E6F946F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="1680" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{4239A55F-B6A0-B74B-A834-7472AF0EB929}"/>
+    <workbookView xWindow="2280" yWindow="1580" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{4239A55F-B6A0-B74B-A834-7472AF0EB929}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
     <sheet name="Groups V0" sheetId="5" r:id="rId2"/>
+    <sheet name="Groups V1" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="72">
   <si>
     <t>spacegroup number</t>
   </si>
@@ -217,28 +218,31 @@
     <t>l = 6n</t>
   </si>
   <si>
-    <t>hexagonal_00</t>
-  </si>
-  <si>
-    <t>hexagonal_01</t>
-  </si>
-  <si>
-    <t>hexagonal_03</t>
-  </si>
-  <si>
-    <t>hexagonal_04</t>
-  </si>
-  <si>
-    <t>hexagonal_05</t>
-  </si>
-  <si>
-    <t>hexagonal_06</t>
-  </si>
-  <si>
-    <t>hexagonal_07</t>
-  </si>
-  <si>
-    <t>hexagonal_08</t>
+    <t>hP_00</t>
+  </si>
+  <si>
+    <t>hP_01</t>
+  </si>
+  <si>
+    <t>hP_03</t>
+  </si>
+  <si>
+    <t>hP_04</t>
+  </si>
+  <si>
+    <t>hP_05</t>
+  </si>
+  <si>
+    <t>hP_06</t>
+  </si>
+  <si>
+    <t>hP_07</t>
+  </si>
+  <si>
+    <t>hP_08</t>
+  </si>
+  <si>
+    <t>hP_02</t>
   </si>
 </sst>
 </file>
@@ -600,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2FEA554-DCE4-B94D-8A39-A08CC83ACBDF}">
   <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:XFD42"/>
+    <sheetView topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1324,8 +1328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B2593AE-0613-FF49-AEF2-84AD3D0B1DD3}">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A33" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2212,4 +2216,871 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97A19A40-4B4E-0D43-870D-492E5DEB1DF2}">
+  <dimension ref="A1:O53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>143</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>147</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>149</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>150</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>156</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6">
+        <v>56</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>157</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>162</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>164</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>168</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>174</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>175</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>177</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>183</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>187</v>
+      </c>
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>189</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>191</v>
+      </c>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>194</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <f>SUM(D2:D18)</f>
+        <v>6300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>144</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21">
+        <v>691</v>
+      </c>
+      <c r="M21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>145</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22">
+        <v>689</v>
+      </c>
+      <c r="M22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>151</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23">
+        <v>39</v>
+      </c>
+      <c r="M23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>152</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24">
+        <v>911</v>
+      </c>
+      <c r="M24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>153</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25">
+        <v>16</v>
+      </c>
+      <c r="M25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>154</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26">
+        <v>699</v>
+      </c>
+      <c r="M26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>171</v>
+      </c>
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27">
+        <v>72</v>
+      </c>
+      <c r="M27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>172</v>
+      </c>
+      <c r="B28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28">
+        <v>54</v>
+      </c>
+      <c r="M28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>180</v>
+      </c>
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29">
+        <v>101</v>
+      </c>
+      <c r="M29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>181</v>
+      </c>
+      <c r="B30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30">
+        <v>54</v>
+      </c>
+      <c r="M30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <f>SUM(D21:D30)</f>
+        <v>3326</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>169</v>
+      </c>
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33">
+        <v>586</v>
+      </c>
+      <c r="M33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>170</v>
+      </c>
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34">
+        <v>552</v>
+      </c>
+      <c r="M34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>178</v>
+      </c>
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35">
+        <v>230</v>
+      </c>
+      <c r="M35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>179</v>
+      </c>
+      <c r="B36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36">
+        <v>202</v>
+      </c>
+      <c r="M36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D37">
+        <f>SUM(D33:D36)</f>
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>158</v>
+      </c>
+      <c r="B39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39">
+        <v>102</v>
+      </c>
+      <c r="H39" t="s">
+        <v>11</v>
+      </c>
+      <c r="I39" t="s">
+        <v>11</v>
+      </c>
+      <c r="M39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>165</v>
+      </c>
+      <c r="B40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40">
+        <v>676</v>
+      </c>
+      <c r="H40" t="s">
+        <v>11</v>
+      </c>
+      <c r="I40" t="s">
+        <v>11</v>
+      </c>
+      <c r="M40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>184</v>
+      </c>
+      <c r="B41" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41">
+        <v>15</v>
+      </c>
+      <c r="H41" t="s">
+        <v>11</v>
+      </c>
+      <c r="I41" t="s">
+        <v>11</v>
+      </c>
+      <c r="M41" t="s">
+        <v>11</v>
+      </c>
+      <c r="N41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>185</v>
+      </c>
+      <c r="B42" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42">
+        <v>96</v>
+      </c>
+      <c r="H42" t="s">
+        <v>11</v>
+      </c>
+      <c r="I42" t="s">
+        <v>11</v>
+      </c>
+      <c r="M42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>188</v>
+      </c>
+      <c r="B43" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" t="s">
+        <v>65</v>
+      </c>
+      <c r="D43">
+        <v>41</v>
+      </c>
+      <c r="H43" t="s">
+        <v>11</v>
+      </c>
+      <c r="I43" t="s">
+        <v>11</v>
+      </c>
+      <c r="M43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>192</v>
+      </c>
+      <c r="B44" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44">
+        <v>120</v>
+      </c>
+      <c r="H44" t="s">
+        <v>11</v>
+      </c>
+      <c r="I44" t="s">
+        <v>11</v>
+      </c>
+      <c r="M44" t="s">
+        <v>11</v>
+      </c>
+      <c r="N44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>193</v>
+      </c>
+      <c r="B45" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" t="s">
+        <v>65</v>
+      </c>
+      <c r="D45">
+        <v>277</v>
+      </c>
+      <c r="H45" t="s">
+        <v>11</v>
+      </c>
+      <c r="I45" t="s">
+        <v>11</v>
+      </c>
+      <c r="M45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>173</v>
+      </c>
+      <c r="B46" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46">
+        <v>914</v>
+      </c>
+      <c r="M46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>176</v>
+      </c>
+      <c r="B47" t="s">
+        <v>42</v>
+      </c>
+      <c r="C47" t="s">
+        <v>65</v>
+      </c>
+      <c r="D47">
+        <v>1461</v>
+      </c>
+      <c r="M47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>182</v>
+      </c>
+      <c r="B48" t="s">
+        <v>48</v>
+      </c>
+      <c r="C48" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48">
+        <v>174</v>
+      </c>
+      <c r="M48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>159</v>
+      </c>
+      <c r="B49" t="s">
+        <v>29</v>
+      </c>
+      <c r="C49" t="s">
+        <v>65</v>
+      </c>
+      <c r="D49">
+        <v>402</v>
+      </c>
+      <c r="M49" t="s">
+        <v>11</v>
+      </c>
+      <c r="N49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>163</v>
+      </c>
+      <c r="B50" t="s">
+        <v>31</v>
+      </c>
+      <c r="C50" t="s">
+        <v>65</v>
+      </c>
+      <c r="D50">
+        <v>459</v>
+      </c>
+      <c r="M50" t="s">
+        <v>11</v>
+      </c>
+      <c r="N50" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>186</v>
+      </c>
+      <c r="B51" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" t="s">
+        <v>65</v>
+      </c>
+      <c r="D51">
+        <v>488</v>
+      </c>
+      <c r="M51" t="s">
+        <v>11</v>
+      </c>
+      <c r="N51" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>190</v>
+      </c>
+      <c r="B52" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52">
+        <v>244</v>
+      </c>
+      <c r="M52" t="s">
+        <v>11</v>
+      </c>
+      <c r="N52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D53">
+        <f>SUM(D39:D52)</f>
+        <v>5469</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>